<commit_message>
All use of Box files removed; added chi-square global
</commit_message>
<xml_diff>
--- a/data/MA/MA_grouped_bar_mut.types.xlsx
+++ b/data/MA/MA_grouped_bar_mut.types.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\Box Sync\Mycoplasma\Experiments\data\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MinimalCell\data\MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5E6DE-B80B-4E55-8AED-9AA9D2C50EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E6C48-3075-4698-B110-BC0714A6F3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19065" yWindow="5910" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="no_large_categ" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>strain</t>
   </si>
@@ -869,10 +870,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306CC8A7-AA13-434B-A564-681023334F80}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <f>D2/SUM($D$2:$D$4)</f>
+        <v>3.3112582781456956E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f>D3/SUM($D$2:$D$4)</f>
+        <v>0.10430463576158941</v>
+      </c>
+      <c r="D3" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <f>D4/SUM($D$2:$D$4)</f>
+        <v>0.86258278145695366</v>
+      </c>
+      <c r="D4" s="1">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <f>D5/SUM(D$5:D$7)</f>
+        <v>2.2648941408173313E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <f>D6/SUM(D$5:D$7)</f>
+        <v>8.6164451009354992E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <f>D7/SUM(D$5:D$7)</f>
+        <v>0.8911866075824717</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1810</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>